<commit_message>
Config parsing (python side)
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">variables</t>
   </si>
   <si>
-    <t xml:space="preserve">__variables</t>
+    <t xml:space="preserve">variables_</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -34,25 +34,25 @@
     <t xml:space="preserve">bands</t>
   </si>
   <si>
-    <t xml:space="preserve">__bands</t>
+    <t xml:space="preserve">bands_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stringmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stringmap_to</t>
   </si>
   <si>
     <t xml:space="preserve">files (no suffix)</t>
   </si>
   <si>
-    <t xml:space="preserve">__location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">__datetime (utc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">__tags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stringmap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">__to</t>
+    <t xml:space="preserve">files_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">files_datetime (utc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">files_tags</t>
   </si>
   <si>
     <t xml:space="preserve">audio_base</t>
@@ -67,21 +67,21 @@
     <t xml:space="preserve">64-0</t>
   </si>
   <si>
+    <t xml:space="preserve">site1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first lake</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1/chunk-20210429_1800</t>
   </si>
   <si>
-    <t xml:space="preserve">site1</t>
-  </si>
-  <si>
     <t xml:space="preserve">20210429_1800</t>
   </si>
   <si>
     <t xml:space="preserve">blue</t>
   </si>
   <si>
-    <t xml:space="preserve">first lake</t>
-  </si>
-  <si>
     <t xml:space="preserve">audio_base_cluster</t>
   </si>
   <si>
@@ -94,16 +94,16 @@
     <t xml:space="preserve">256-0</t>
   </si>
   <si>
+    <t xml:space="preserve">site2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strange lake</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1/chunk-20210429_1801</t>
   </si>
   <si>
     <t xml:space="preserve">20210429_1801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strange lake</t>
   </si>
   <si>
     <t xml:space="preserve">audio_expected_sample_rate</t>
@@ -384,8 +384,8 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8:J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,11 +394,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="2.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="2.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="2.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,22 +418,22 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="0" t="s">
@@ -443,7 +444,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -463,23 +464,23 @@
       <c r="E3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>19</v>
@@ -501,26 +502,26 @@
       <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="0" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="0" t="s">
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="K4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="M4" s="0" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,20 +540,20 @@
       <c r="E5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>18</v>
+      <c r="M5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,20 +572,20 @@
       <c r="E6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="K6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>18</v>
+      <c r="M6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,30 +599,30 @@
       <c r="E7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>18</v>
+      <c r="M7" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -633,19 +634,19 @@
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="K9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -659,19 +660,19 @@
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="K10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -679,19 +680,19 @@
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="K11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="M11" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -705,19 +706,19 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="K12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="M12" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -725,27 +726,28 @@
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="K13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="M13" s="0" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -753,7 +755,7 @@
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -761,7 +763,7 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -769,7 +771,7 @@
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -777,10 +779,10 @@
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="0" t="s">
+      <c r="I18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>55</v>
       </c>
     </row>
@@ -788,10 +790,10 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="0" t="s">
+      <c r="I19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="0" t="s">
         <v>56</v>
       </c>
     </row>
@@ -799,7 +801,7 @@
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -807,7 +809,7 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -815,7 +817,7 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -823,7 +825,7 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -831,7 +833,7 @@
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -839,7 +841,7 @@
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -847,7 +849,7 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -855,7 +857,7 @@
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -863,7 +865,7 @@
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -871,7 +873,7 @@
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -879,7 +881,7 @@
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -887,7 +889,7 @@
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -895,7 +897,7 @@
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -903,7 +905,7 @@
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -911,7 +913,7 @@
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -919,7 +921,7 @@
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -927,7 +929,7 @@
       <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature extractor + spectrogram previewer, per band
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="62">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">audio_base</t>
   </si>
   <si>
-    <t xml:space="preserve">./sample/audio</t>
+    <t xml:space="preserve">./audio/</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">feature_base</t>
   </si>
   <si>
-    <t xml:space="preserve">/run/media/twilight/My Passport/mozambique/2021-06-24-09h49-mozambique-test/</t>
+    <t xml:space="preserve">./features/</t>
   </si>
   <si>
     <t xml:space="preserve">log2/chunk-20210429_1800</t>
@@ -163,28 +163,43 @@
     <t xml:space="preserve">green</t>
   </si>
   <si>
+    <t xml:space="preserve">generated_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./generated/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preview_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preview_file_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preview_file_dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green,windy</t>
+  </si>
+  <si>
     <t xml:space="preserve">integration_seconds</t>
   </si>
   <si>
     <t xml:space="preserve">30-60-180-300</t>
   </si>
   <si>
-    <t xml:space="preserve">log2/chunk-20210429_1801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_1802</t>
-  </si>
-  <si>
     <t xml:space="preserve">display_in_utc_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_1803</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_1810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green,windy</t>
   </si>
   <si>
     <t xml:space="preserve">idea: use @location@/chunk-@datetime@</t>
@@ -284,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,6 +317,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,8 +403,8 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -677,6 +696,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
@@ -684,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>24</v>
@@ -697,12 +722,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>2</v>
-      </c>
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
@@ -710,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>24</v>
@@ -723,6 +746,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -730,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>24</v>
@@ -739,11 +766,16 @@
         <v>42</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
+      <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>58</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
@@ -760,6 +792,12 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
@@ -776,6 +814,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
@@ -783,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Command to print frequency bounds for the bands
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -725,7 +725,9 @@
       <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
@@ -749,7 +751,9 @@
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="n">
+        <v>20</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Start integrating preview in the vue project
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -88,61 +88,61 @@
     <t xml:space="preserve">/home_expes/mozambique2021AvrilMai/Soundscapes MSR/</t>
   </si>
   <si>
+    <t xml:space="preserve">band4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256-192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strange lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_1801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_expected_sample_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256-128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.WAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_1803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1803</t>
+  </si>
+  <si>
     <t xml:space="preserve">band1</t>
   </si>
   <si>
     <t xml:space="preserve">256-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strange lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_1801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_1801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_expected_sample_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_1802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_1802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_suffix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00.WAV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256-128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_1803</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_1803</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256-192</t>
   </si>
   <si>
     <t xml:space="preserve">log1/chunk-20210429_1810</t>
@@ -299,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -309,6 +309,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,7 +408,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,6 +418,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="2.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="2.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15"/>
@@ -440,7 +445,7 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -486,7 +491,7 @@
       <c r="G3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -498,7 +503,7 @@
       <c r="K3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="0" t="s">
@@ -509,7 +514,7 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -518,13 +523,13 @@
       <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -536,7 +541,7 @@
       <c r="K4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="0" t="s">
@@ -568,7 +573,7 @@
       <c r="K5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="0" t="s">
@@ -600,7 +605,7 @@
       <c r="K6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="0" t="s">
@@ -615,7 +620,7 @@
       <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -627,7 +632,7 @@
       <c r="K7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M7" s="0" t="s">
@@ -641,7 +646,7 @@
       <c r="I8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -662,7 +667,7 @@
       <c r="K9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M9" s="0" t="s">
@@ -688,7 +693,7 @@
       <c r="K10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="0" t="s">
@@ -696,10 +701,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -714,7 +719,7 @@
       <c r="K11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M11" s="0" t="s">
@@ -722,11 +727,11 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>0</v>
+      <c r="B12" s="4" t="n">
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -740,7 +745,7 @@
       <c r="K12" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="M12" s="0" t="s">
@@ -748,11 +753,11 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>20</v>
+      <c r="B13" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -766,7 +771,7 @@
       <c r="K13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="4" t="s">
         <v>42</v>
       </c>
       <c r="M13" s="0" t="s">

</xml_diff>

<commit_message>
Remove the use of a default preview_file
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -701,7 +701,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="4" t="s">

</xml_diff>

<commit_message>
Generate extract with ffmpeg incl. ultrasound magnifier
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -196,7 +196,13 @@
     <t xml:space="preserve">integration_seconds</t>
   </si>
   <si>
-    <t xml:space="preserve">30-60-180-300</t>
+    <t xml:space="preserve">600-1800-3600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nearest_radiuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">025-050-075-100-125-150</t>
   </si>
   <si>
     <t xml:space="preserve">display_in_utc_plus</t>
@@ -408,7 +414,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,6 +799,12 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
@@ -801,12 +813,6 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
@@ -815,6 +821,12 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
@@ -823,7 +835,6 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
@@ -831,10 +842,11 @@
         <v>2</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
@@ -842,7 +854,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Expect and load timeranges from the xlsx file
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="70">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">stringmap_to</t>
   </si>
   <si>
+    <t xml:space="preserve">timeranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeranges_</t>
+  </si>
+  <si>
     <t xml:space="preserve">files (no suffix)</t>
   </si>
   <si>
@@ -73,6 +79,12 @@
     <t xml:space="preserve">first lake</t>
   </si>
   <si>
+    <t xml:space="preserve">first4min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1800-20210429_1804</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1/chunk-20210429_1800</t>
   </si>
   <si>
@@ -98,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">strange lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1810-20210429_1811</t>
   </si>
   <si>
     <t xml:space="preserve">log1/chunk-20210429_1801</t>
@@ -305,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,15 +340,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,25 +433,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="2.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="2.49"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="2.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,109 +479,127 @@
       <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>19</v>
+      <c r="O3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>192000</v>
@@ -565,57 +608,57 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,191 +667,191 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="L8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>46</v>
+      <c r="L9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>46</v>
+      <c r="L10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>46</v>
+      <c r="L11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" s="6" t="n">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>56</v>
+      <c r="L13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -816,13 +859,13 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2</v>
@@ -830,7 +873,7 @@
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -838,11 +881,11 @@
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>62</v>
+      <c r="L18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,18 +893,18 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>63</v>
+      <c r="L19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -869,7 +912,7 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -877,7 +920,7 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -885,7 +928,7 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -893,7 +936,7 @@
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -901,7 +944,7 @@
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -909,7 +952,7 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -917,7 +960,7 @@
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -925,7 +968,7 @@
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -933,7 +976,7 @@
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -941,7 +984,7 @@
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -949,7 +992,7 @@
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -957,7 +1000,7 @@
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -965,7 +1008,7 @@
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -973,7 +1016,7 @@
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -981,7 +1024,7 @@
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -989,7 +1032,7 @@
       <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve config parsing + start work around umap
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="88">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -37,16 +37,34 @@
     <t xml:space="preserve">bands_</t>
   </si>
   <si>
+    <t xml:space="preserve">umaps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umaps_integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umaps_bands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umaps_ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umaps_sites</t>
+  </si>
+  <si>
     <t xml:space="preserve">stringmap</t>
   </si>
   <si>
     <t xml:space="preserve">stringmap_to</t>
   </si>
   <si>
-    <t xml:space="preserve">timeranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeranges_</t>
+    <t xml:space="preserve">stringmap_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges_</t>
   </si>
   <si>
     <t xml:space="preserve">files (no suffix)</t>
@@ -73,12 +91,27 @@
     <t xml:space="preserve">64-0</t>
   </si>
   <si>
+    <t xml:space="preserve">u_1min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all,band2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first4min,min10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site1,site2</t>
+  </si>
+  <si>
     <t xml:space="preserve">site1</t>
   </si>
   <si>
     <t xml:space="preserve">first lake</t>
   </si>
   <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
     <t xml:space="preserve">first4min</t>
   </si>
   <si>
@@ -91,9 +124,6 @@
     <t xml:space="preserve">20210429_1800</t>
   </si>
   <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
     <t xml:space="preserve">audio_base_cluster</t>
   </si>
   <si>
@@ -106,12 +136,18 @@
     <t xml:space="preserve">256-192</t>
   </si>
   <si>
+    <t xml:space="preserve">u_2min</t>
+  </si>
+  <si>
     <t xml:space="preserve">site2</t>
   </si>
   <si>
     <t xml:space="preserve">strange lake</t>
   </si>
   <si>
+    <t xml:space="preserve">#9632ff</t>
+  </si>
+  <si>
     <t xml:space="preserve">min10</t>
   </si>
   <si>
@@ -133,6 +169,9 @@
     <t xml:space="preserve">256-128</t>
   </si>
   <si>
+    <t xml:space="preserve">4 minutes taken at 18:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1/chunk-20210429_1802</t>
   </si>
   <si>
@@ -151,6 +190,9 @@
     <t xml:space="preserve">256-64</t>
   </si>
   <si>
+    <t xml:space="preserve">1 minute at 18:10</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1/chunk-20210429_1803</t>
   </si>
   <si>
@@ -190,25 +232,46 @@
     <t xml:space="preserve">log2/chunk-20210429_1801</t>
   </si>
   <si>
+    <t xml:space="preserve">other_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./other/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_1803</t>
+  </si>
+  <si>
     <t xml:space="preserve">preview_file</t>
   </si>
   <si>
-    <t xml:space="preserve">log2/chunk-20210429_1802</t>
+    <t xml:space="preserve">log2/chunk-20210429_1810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green,windy</t>
   </si>
   <si>
     <t xml:space="preserve">preview_file_start</t>
   </si>
   <si>
-    <t xml:space="preserve">log2/chunk-20210429_1803</t>
-  </si>
-  <si>
     <t xml:space="preserve">preview_file_dur</t>
   </si>
   <si>
-    <t xml:space="preserve">log2/chunk-20210429_1810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green,windy</t>
+    <t xml:space="preserve">display_in_utc_plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idea: use @location@/chunk-@datetime@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa/Maputo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or @location@/%y%M%d_……. (preproc + strftime)</t>
   </si>
   <si>
     <t xml:space="preserve">integration_seconds</t>
@@ -221,15 +284,6 @@
   </si>
   <si>
     <t xml:space="preserve">025-050-075-100-125-150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_in_utc_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idea: use @location@/chunk-@datetime@</t>
-  </si>
-  <si>
-    <t xml:space="preserve">or @location@/%y%M%d_……. (preproc + strftime)</t>
   </si>
 </sst>
 </file>
@@ -323,7 +377,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,6 +403,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,10 +491,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,15 +504,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="2.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="2.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="11.54"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="2.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="10" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="2.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="2.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,133 +535,199 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="O1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>120</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="M4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="V4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>192000</v>
@@ -608,57 +736,76 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="M5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>23</v>
+      <c r="N6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,260 +814,321 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="6"/>
+      <c r="P8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>52</v>
+      <c r="P9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>52</v>
+      <c r="P10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>52</v>
+      <c r="P11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="W12" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="6" t="n">
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P13" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="P15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="P16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="P17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>68</v>
+      <c r="P18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U18" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
+      <c r="A19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N19" s="0" t="s">
-        <v>69</v>
+      <c r="P19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="P20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="P21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>87</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="P22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -928,7 +1136,10 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="P23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -936,7 +1147,10 @@
       <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="P24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -944,7 +1158,10 @@
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="P25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -952,7 +1169,10 @@
       <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="P26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -960,7 +1180,10 @@
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="P27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -968,7 +1191,10 @@
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="P28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -976,7 +1202,10 @@
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="P29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -984,7 +1213,10 @@
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="P30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -992,7 +1224,10 @@
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="P31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1000,7 +1235,10 @@
       <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="P32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1008,7 +1246,10 @@
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="P33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1016,7 +1257,10 @@
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="P34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1024,7 +1268,10 @@
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="P35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1032,7 +1279,10 @@
       <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="P36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S36" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1040,24 +1290,39 @@
       <c r="C37" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="P37" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="P38" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="P39" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="P40" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P41" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate umap json and possibly the scatter plots
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="89">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">files_location</t>
   </si>
   <si>
-    <t xml:space="preserve">files_datetime (utc)</t>
+    <t xml:space="preserve">files_start (utc)</t>
   </si>
   <si>
     <t xml:space="preserve">files_tags</t>
@@ -169,6 +169,12 @@
     <t xml:space="preserve">256-128</t>
   </si>
   <si>
+    <t xml:space="preserve">u_10sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band2</t>
+  </si>
+  <si>
     <t xml:space="preserve">4 minutes taken at 18:00</t>
   </si>
   <si>
@@ -182,9 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">00.WAV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band2</t>
   </si>
   <si>
     <t xml:space="preserve">256-64</t>
@@ -493,8 +496,8 @@
   </sheetPr>
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -741,12 +744,26 @@
       <c r="E5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>2</v>
@@ -755,13 +772,13 @@
         <v>2</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>27</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="W5" s="0" t="s">
         <v>29</v>
@@ -769,25 +786,25 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>2</v>
@@ -796,13 +813,13 @@
         <v>2</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>27</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W6" s="0" t="s">
         <v>29</v>
@@ -814,10 +831,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>2</v>
@@ -826,13 +843,13 @@
         <v>2</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>27</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="W7" s="0" t="s">
         <v>29</v>
@@ -852,10 +869,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -867,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>39</v>
@@ -876,15 +893,15 @@
         <v>33</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -896,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>39</v>
@@ -905,15 +922,15 @@
         <v>45</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -925,16 +942,16 @@
         <v>2</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,24 +965,24 @@
         <v>2</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>39</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -977,21 +994,21 @@
         <v>2</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>50</v>
@@ -1008,7 +1025,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>10</v>
@@ -1048,7 +1065,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2</v>
@@ -1063,15 +1080,15 @@
         <v>2</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
@@ -1083,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,10 +1117,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
@@ -1117,10 +1134,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fix grouping by site for umap
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="90">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -172,22 +172,25 @@
     <t xml:space="preserve">u_10sec</t>
   </si>
   <si>
+    <t xml:space="preserve">all,band4,band3,band2,band1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 minutes taken at 18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.WAV</t>
+  </si>
+  <si>
     <t xml:space="preserve">band2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 minutes taken at 18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_1802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_1802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_suffix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00.WAV</t>
   </si>
   <si>
     <t xml:space="preserve">256-64</t>
@@ -497,7 +500,7 @@
   <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -795,16 +798,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>2</v>
@@ -813,13 +816,13 @@
         <v>2</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>27</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W6" s="0" t="s">
         <v>29</v>
@@ -831,10 +834,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>2</v>
@@ -843,13 +846,13 @@
         <v>2</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>27</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="W7" s="0" t="s">
         <v>29</v>
@@ -869,10 +872,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -884,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>39</v>
@@ -893,15 +896,15 @@
         <v>33</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -913,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>39</v>
@@ -922,15 +925,15 @@
         <v>45</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -942,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="U11" s="0" t="s">
         <v>39</v>
@@ -951,7 +954,7 @@
         <v>53</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,24 +968,24 @@
         <v>2</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>39</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -994,21 +997,21 @@
         <v>2</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>50</v>
@@ -1025,7 +1028,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>10</v>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2</v>
@@ -1080,15 +1083,15 @@
         <v>2</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
@@ -1100,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,10 +1120,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
@@ -1134,10 +1137,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Switch to site (instead of loc) + add tool (py) to look at recording times
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">files (no suffix)</t>
   </si>
   <si>
-    <t xml:space="preserve">files_location</t>
+    <t xml:space="preserve">files_site</t>
   </si>
   <si>
     <t xml:space="preserve">files_start (utc)</t>
@@ -300,7 +300,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -328,11 +328,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -383,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,15 +399,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,11 +490,11 @@
   </sheetPr>
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
@@ -516,7 +507,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="2.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="24.6"/>
@@ -703,7 +694,7 @@
       <c r="N4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="P4" s="2" t="s">
@@ -836,7 +827,7 @@
       <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P7" s="2" t="s">

</xml_diff>

<commit_message>
Refactor grouping involved in umap to start volume computation
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -19,6 +19,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Used currently for the mock volume
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="90">
   <si>
@@ -300,7 +324,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -325,6 +349,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -378,7 +410,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,6 +440,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,7 +510,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -490,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
@@ -507,7 +543,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="2.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="1.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="24.6"/>
@@ -1058,7 +1094,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -1127,7 +1163,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -1355,5 +1391,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generating different per range volumes
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -19,30 +19,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="A21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Used currently for the mock volume
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="90">
   <si>
@@ -307,7 +283,7 @@
     <t xml:space="preserve">integration_seconds</t>
   </si>
   <si>
-    <t xml:space="preserve">600-1800-3600</t>
+    <t xml:space="preserve">60-120-10</t>
   </si>
   <si>
     <t xml:space="preserve">nearest_radiuses</t>
@@ -1391,6 +1367,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of Readme + reset of config.xlsx
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">audio_base</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/emilien/git/sound-scape-explorer/sample/audio/BORA_ANR_sons</t>
+    <t xml:space="preserve">../sample/audio/BORA_ANR_sons</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">feature_base</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/emilien/git/sound-scape-explorer/sample/features</t>
+    <t xml:space="preserve">../sample/features</t>
   </si>
   <si>
     <t xml:space="preserve">^ pas utilisé, pourrait servir à choisir</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">generated_base</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/emilien/git/sound-scape-explorer/sample/generated/</t>
+    <t xml:space="preserve">../sample/generated/</t>
   </si>
   <si>
     <t xml:space="preserve">couleur etc</t>
@@ -3637,10 +3637,10 @@
   <dimension ref="A1:Y530"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>

</xml_diff>

<commit_message>
Adding player.vue + edit of config.xlsx + Logger Classes
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -232,7 +232,7 @@
     <t xml:space="preserve">feature_base</t>
   </si>
   <si>
-    <t xml:space="preserve">../sample/features</t>
+    <t xml:space="preserve">./features</t>
   </si>
   <si>
     <t xml:space="preserve">^ pas utilisé, pourrait servir à choisir</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">generated_base</t>
   </si>
   <si>
-    <t xml:space="preserve">../sample/generated/</t>
+    <t xml:space="preserve">./generated/</t>
   </si>
   <si>
     <t xml:space="preserve">couleur etc</t>
@@ -3637,10 +3637,10 @@
   <dimension ref="A1:Y530"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>

</xml_diff>

<commit_message>
Example version more slight + readme updates ( md->html )
</commit_message>
<xml_diff>
--- a/sample/config.xlsx
+++ b/sample/config.xlsx
@@ -636,11 +636,11 @@
   </sheetPr>
   <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T20" activeCellId="1" sqref="W3 T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>

</xml_diff>